<commit_message>
ETL stage x historico
</commit_message>
<xml_diff>
--- a/00Entrada/17022022_2JR_Multimarcas.xlsx
+++ b/00Entrada/17022022_2JR_Multimarcas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01Projeto\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EasyDash\00Entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AD9FE9F-EE7D-405B-AB02-725C4153B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88AD99B-2372-470D-B623-E67E32923A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B12BC72C-8DA8-4F11-923B-E0B0078FE7F7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="91">
   <si>
     <t>Data</t>
   </si>
@@ -660,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A902DF2-735F-4D84-B25E-6B05F4EBCC71}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,19 +730,19 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44611</v>
+        <v>44609</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>54234</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>84212</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -760,23 +760,23 @@
         <v>80</v>
       </c>
       <c r="K2">
-        <f>SUM(I2-J2)</f>
+        <f t="shared" ref="K2:K26" si="0">SUM(I2-J2)</f>
         <v>120</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N2">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>54234</v>
+        <v>44454</v>
       </c>
       <c r="D3">
         <v>84212</v>
@@ -799,20 +799,20 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I3">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="J3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K27" si="0">SUM(I3-J3)</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>110</v>
       </c>
       <c r="L3">
         <v>4</v>
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>44454</v>
+        <v>12124</v>
       </c>
       <c r="D4">
         <v>84212</v>
@@ -847,23 +847,23 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I4">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="J4">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>40</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -886,50 +886,50 @@
         <v>44609</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>11234</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>300</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="L5">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>12124</v>
-      </c>
-      <c r="D5">
-        <v>84212</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5">
-        <v>70</v>
-      </c>
-      <c r="J5">
+      <c r="M5" t="s">
         <v>30</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="M5" t="s">
-        <v>20</v>
-      </c>
       <c r="N5">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -937,47 +937,47 @@
         <v>44609</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>11234</v>
+        <v>54234</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>69421</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="I6">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="J6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="N6">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="P6" t="s">
         <v>19</v>
@@ -991,7 +991,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>54234</v>
+        <v>33125</v>
       </c>
       <c r="D7">
         <v>69421</v>
@@ -1000,23 +1000,23 @@
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="I7">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="J7">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -1042,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>33125</v>
+        <v>12513</v>
       </c>
       <c r="D8">
         <v>69421</v>
@@ -1051,23 +1051,23 @@
         <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
         <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8">
+        <v>250</v>
+      </c>
+      <c r="J8">
         <v>120</v>
       </c>
-      <c r="J8">
-        <v>50</v>
-      </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="L8">
         <v>5</v>
@@ -1090,50 +1090,50 @@
         <v>44609</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>12513</v>
+        <v>98123</v>
       </c>
       <c r="D9">
-        <v>69421</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I9">
-        <v>250</v>
+        <v>90</v>
       </c>
       <c r="J9">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="L9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M9" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="N9">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s">
         <v>18</v>
       </c>
       <c r="P9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1141,10 +1141,10 @@
         <v>44609</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>98123</v>
+        <v>98124</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1159,32 +1159,32 @@
         <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I10">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="J10">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="L10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N10">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="O10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="P10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1192,10 +1192,10 @@
         <v>44609</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>98124</v>
+        <v>52349</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1204,35 +1204,35 @@
         <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="I11">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J11">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M11" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="N11">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="O11" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
         <v>19</v>
@@ -1243,10 +1243,10 @@
         <v>44609</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>52349</v>
+        <v>52350</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1255,38 +1255,38 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I12">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J12">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M12" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="N12">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1294,10 +1294,10 @@
         <v>44609</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>52350</v>
+        <v>52351</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1306,35 +1306,35 @@
         <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="I13">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J13">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L13">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="M13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="P13" t="s">
         <v>22</v>
@@ -1345,10 +1345,10 @@
         <v>44609</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>52351</v>
+        <v>52352</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1360,35 +1360,35 @@
         <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I14">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J14">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="N14">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O14" t="s">
         <v>21</v>
       </c>
       <c r="P14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1396,16 +1396,16 @@
         <v>44609</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>52352</v>
+        <v>52353</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>45213</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F15" t="s">
         <v>45</v>
@@ -1414,29 +1414,29 @@
         <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I15">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J15">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L15">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M15" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="N15">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O15" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
       <c r="P15" t="s">
         <v>19</v>
@@ -1447,10 +1447,10 @@
         <v>44609</v>
       </c>
       <c r="B16">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>52353</v>
+        <v>52354</v>
       </c>
       <c r="D16">
         <v>45213</v>
@@ -1459,35 +1459,35 @@
         <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16">
+        <v>136</v>
+      </c>
+      <c r="J16">
+        <v>66</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="L16">
+        <v>36</v>
+      </c>
+      <c r="M16" t="s">
+        <v>78</v>
+      </c>
+      <c r="N16">
         <v>23</v>
       </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16">
-        <v>135</v>
-      </c>
-      <c r="J16">
-        <v>65</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="L16">
-        <v>35</v>
-      </c>
-      <c r="M16" t="s">
-        <v>77</v>
-      </c>
-      <c r="N16">
-        <v>22</v>
-      </c>
       <c r="O16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P16" t="s">
         <v>19</v>
@@ -1498,10 +1498,10 @@
         <v>44609</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17">
-        <v>52354</v>
+        <v>52355</v>
       </c>
       <c r="D17">
         <v>45213</v>
@@ -1513,29 +1513,29 @@
         <v>54</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="I17">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J17">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L17">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N17">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O17" t="s">
         <v>88</v>
@@ -1549,50 +1549,50 @@
         <v>44609</v>
       </c>
       <c r="B18">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18">
-        <v>52355</v>
+        <v>52356</v>
       </c>
       <c r="D18">
-        <v>45213</v>
+        <v>32145</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I18">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J18">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L18">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O18" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="P18" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1600,47 +1600,47 @@
         <v>44609</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19">
-        <v>52356</v>
+        <v>52357</v>
       </c>
       <c r="D19">
-        <v>32145</v>
+        <v>21345</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="H19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I19">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J19">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L19">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="P19" t="s">
         <v>22</v>
@@ -1651,50 +1651,50 @@
         <v>44609</v>
       </c>
       <c r="B20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20">
-        <v>52357</v>
+        <v>52358</v>
       </c>
       <c r="D20">
-        <v>21345</v>
+        <v>32145</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
         <v>45</v>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I20">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J20">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L20">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N20">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O20" t="s">
         <v>18</v>
       </c>
       <c r="P20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1702,50 +1702,50 @@
         <v>44609</v>
       </c>
       <c r="B21">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21">
-        <v>52358</v>
+        <v>52359</v>
       </c>
       <c r="D21">
-        <v>32145</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
         <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I21">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J21">
+        <v>71</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
       <c r="L21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O21" t="s">
         <v>18</v>
       </c>
       <c r="P21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -1753,10 +1753,10 @@
         <v>44609</v>
       </c>
       <c r="B22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22">
-        <v>52359</v>
+        <v>52360</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1771,32 +1771,32 @@
         <v>57</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I22">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O22" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="P22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1804,10 +1804,10 @@
         <v>44609</v>
       </c>
       <c r="B23">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23">
-        <v>52360</v>
+        <v>52361</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1816,35 +1816,35 @@
         <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H23" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23">
+        <v>143</v>
+      </c>
+      <c r="J23">
+        <v>73</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="I23">
-        <v>142</v>
-      </c>
-      <c r="J23">
-        <v>72</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
       <c r="L23">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M23" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N23">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P23" t="s">
         <v>19</v>
@@ -1855,47 +1855,47 @@
         <v>44609</v>
       </c>
       <c r="B24">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24">
-        <v>52361</v>
+        <v>52362</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>54622</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I24">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J24">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="L24">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="M24" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="N24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O24" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="P24" t="s">
         <v>19</v>
@@ -1906,10 +1906,10 @@
         <v>44609</v>
       </c>
       <c r="B25">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>52362</v>
+        <v>52363</v>
       </c>
       <c r="D25">
         <v>54622</v>
@@ -1918,19 +1918,19 @@
         <v>40</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
         <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I25">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J25">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
@@ -1943,7 +1943,7 @@
         <v>17</v>
       </c>
       <c r="N25">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O25" t="s">
         <v>18</v>
@@ -1957,31 +1957,31 @@
         <v>44609</v>
       </c>
       <c r="B26">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>52363</v>
+        <v>52364</v>
       </c>
       <c r="D26">
-        <v>54622</v>
+        <v>84212</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G26" t="s">
         <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I26">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J26">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
@@ -1994,63 +1994,12 @@
         <v>17</v>
       </c>
       <c r="N26">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O26" t="s">
         <v>18</v>
       </c>
       <c r="P26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>44609</v>
-      </c>
-      <c r="B27">
-        <v>22</v>
-      </c>
-      <c r="C27">
-        <v>52364</v>
-      </c>
-      <c r="D27">
-        <v>84212</v>
-      </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>74</v>
-      </c>
-      <c r="I27">
-        <v>146</v>
-      </c>
-      <c r="J27">
-        <v>76</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="L27">
-        <v>44</v>
-      </c>
-      <c r="M27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N27">
-        <v>33</v>
-      </c>
-      <c r="O27" t="s">
-        <v>18</v>
-      </c>
-      <c r="P27" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>